<commit_message>
e commerce test cases
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darsh\Desktop\manual-testing-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A26803-25F2-423E-8F72-396C1F04B4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581CE120-A258-4805-8520-26E38018E6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{52B6C61F-30E7-4B0C-9B6E-4F8256513974}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="172">
   <si>
     <t>TestCases</t>
   </si>
@@ -287,13 +287,373 @@
   </si>
   <si>
     <t>Page struck with no message</t>
+  </si>
+  <si>
+    <t>Verify search with valid product name</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>Verify seach with partial product name</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>Verify search with blank input</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>Verify search suggestions when typing</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>Cart Module:</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t>TC017</t>
+  </si>
+  <si>
+    <t>TC018</t>
+  </si>
+  <si>
+    <t>TC019</t>
+  </si>
+  <si>
+    <t>TC020</t>
+  </si>
+  <si>
+    <t>Checkout Module:</t>
+  </si>
+  <si>
+    <t>TC0021</t>
+  </si>
+  <si>
+    <t>TC0022</t>
+  </si>
+  <si>
+    <t>TC0023</t>
+  </si>
+  <si>
+    <t>TC0024</t>
+  </si>
+  <si>
+    <t>TC0025</t>
+  </si>
+  <si>
+    <t>TC0026</t>
+  </si>
+  <si>
+    <t>TC0027</t>
+  </si>
+  <si>
+    <t>TC0028</t>
+  </si>
+  <si>
+    <t>TC0029</t>
+  </si>
+  <si>
+    <t>TC0030</t>
+  </si>
+  <si>
+    <t>User should have valid credentials</t>
+  </si>
+  <si>
+    <t>1. Login to the website with valid credentials. 
+2. In the search tab, search with valid product names.</t>
+  </si>
+  <si>
+    <t>User should see similar products after searching</t>
+  </si>
+  <si>
+    <t>1. Login to the website with valid credentials. 
+2. In the search tab, search with valid partial product names.</t>
+  </si>
+  <si>
+    <t>Product name: Shoes/Bottles/ Bag</t>
+  </si>
+  <si>
+    <t>Product name: bott/ tow/ mob</t>
+  </si>
+  <si>
+    <t>1. Login to the website with valid credentials. 
+2. In the search tab don’t enter anything, search blank input</t>
+  </si>
+  <si>
+    <t>User should see home page refreshing everytime when searched with blank input</t>
+  </si>
+  <si>
+    <t>Homepage has no changes</t>
+  </si>
+  <si>
+    <t>1. Login to the website with valid credentials. 
+2. In the search tab, start typing any product and observe the suggestions</t>
+  </si>
+  <si>
+    <t>User is logged in and on the search results page</t>
+  </si>
+  <si>
+    <t>Verify filtering of search results by category</t>
+  </si>
+  <si>
+    <t>Product: Laptop
+Brand: dell</t>
+  </si>
+  <si>
+    <t>1. Enter a valid keyword in the search bar and click on Search.
+2. On the results page, select a filter.
+3. Observe the updated search results.</t>
+  </si>
+  <si>
+    <r>
+      <t>Only products matching the filter criteria (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dell Laptops</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) should be displayed</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see similar product search  suggestions </t>
+  </si>
+  <si>
+    <t>Verify sorting of search results by price (Low → High)</t>
+  </si>
+  <si>
+    <t>1. Search for Mobile Phones.
+2. On the results page, select Sort by Price: Low to High.
+3. Observe the order of items.</t>
+  </si>
+  <si>
+    <t>Product: Mobile</t>
+  </si>
+  <si>
+    <t>Products should be sorted from lowest price to highest price.</t>
+  </si>
+  <si>
+    <t>Verify user can add product to the cart</t>
+  </si>
+  <si>
+    <t>User is in home page after login</t>
+  </si>
+  <si>
+    <t>1. Add products to the cart by clicking on 'Add to cart' CTA. 
+2. Click on cart icon and observe the cart page</t>
+  </si>
+  <si>
+    <t>User should be able to see the added products in cart page</t>
+  </si>
+  <si>
+    <t>Verify product quantity can be updated in the cart</t>
+  </si>
+  <si>
+    <t>1. Add products to the cart by clicking on 'Add to cart' CTA. 
+2. Click on cart icon and observe the cart page.
+3. Click on '+' CTA to increase the quantity of the products</t>
+  </si>
+  <si>
+    <t>After clicking on '+' CTA the quantity of the product should increase</t>
+  </si>
+  <si>
+    <t>The product quantity is not increasing.</t>
+  </si>
+  <si>
+    <t>Verify products can be removed from the cart.</t>
+  </si>
+  <si>
+    <t>1. Add products to the cart by clicking on 'Add to cart' CTA. 
+2. Click on cart icon and land on the cart page.
+3. Click on 'delete' CTA beside the products and observe.</t>
+  </si>
+  <si>
+    <t>The products should be removed from the cart page after clicking on 'delete' CTA</t>
+  </si>
+  <si>
+    <t>Verify total price of the cart changes when products are added.</t>
+  </si>
+  <si>
+    <t>1. Add products to the cart by clicking on 'Add to cart' CTA. 
+2. Click on cart icon and observe the cart page.
+3. Click on '+' CTA to increase the quantity of the products.
+4. Observe the price in the cart page</t>
+  </si>
+  <si>
+    <t>The price of the product should increase</t>
+  </si>
+  <si>
+    <t>Verify cart persists after logout and login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add products to the cart by clicking on 'Add to cart' CTA.
+2. Now go back to home page and Logout of the application.
+3. Again Login with the same credentials to the application.
+4. Go to cart page and check for the added products in the cart </t>
+  </si>
+  <si>
+    <t>User should see the previously added products in the cart</t>
+  </si>
+  <si>
+    <t>Verify user can proceed to checkout with products in the cart.</t>
+  </si>
+  <si>
+    <t>Verify billing and shipping address fields are mandatory.</t>
+  </si>
+  <si>
+    <t>Verify order confirmation page is displayed after successful payment.</t>
+  </si>
+  <si>
+    <t>User logged in, at least one product in cart</t>
+  </si>
+  <si>
+    <t>1. Go to Cart
+2. Click Checkout
+3. Enter valid shipping details
+4. Select a valid payment method
+5. Place order</t>
+  </si>
+  <si>
+    <t>1. Go to Cart
+2. Click Checkout
+3. Leave blank fields for shipping address.
+4. Click on continue</t>
+  </si>
+  <si>
+    <t>User cannot proceed further unless the shipping details are filled. Error is shown</t>
+  </si>
+  <si>
+    <t>Error is shown as 'Please enter the shipping details'</t>
+  </si>
+  <si>
+    <t>User logged in, empty cart</t>
+  </si>
+  <si>
+    <t>1. Navigate to Checkout page directly</t>
+  </si>
+  <si>
+    <t>System should block checkout and show “Your cart is empty” message</t>
+  </si>
+  <si>
+    <t>Verify user cannot proceed to checkout without products in the cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify multiple payment options </t>
+  </si>
+  <si>
+    <t>1. Go to Checkout
+2. Check available payment options (Card/UPI/NetBanking/Wallets/COD)
+3. Try placing order with each</t>
+  </si>
+  <si>
+    <t>Payment options available and order placed successfully for each valid method</t>
+  </si>
+  <si>
+    <t>Verify error for invalid card details.</t>
+  </si>
+  <si>
+    <t>1. Go to Checkout
+2. Select “Credit Card”
+3. Enter invalid card number or expired date
+4. Click Pay</t>
+  </si>
+  <si>
+    <t>Card: 1112325636141
+cvv: 112</t>
+  </si>
+  <si>
+    <t>Payment should fail with proper error message "Invalid Card "/ "Payment Failed"</t>
+  </si>
+  <si>
+    <t>Verify Select payment method (Credit Card)</t>
+  </si>
+  <si>
+    <t>User is on payment page</t>
+  </si>
+  <si>
+    <t>1. Select "Credit Card" option
+2. Enter valid card details
+3. Click "Pay Now"</t>
+  </si>
+  <si>
+    <t>Payment should be processed successfully</t>
+  </si>
+  <si>
+    <t>Error "Payment gateway is under maintenance"</t>
+  </si>
+  <si>
+    <t>Verify valid discount coupon</t>
+  </si>
+  <si>
+    <t>User has items in cart and a valid coupon code</t>
+  </si>
+  <si>
+    <t>1. Navigate to checkout
+2. Enter valid coupon code
+3. Apply coupon</t>
+  </si>
+  <si>
+    <t>Discount should be applied to the total amount</t>
+  </si>
+  <si>
+    <t>Coupon service is down</t>
+  </si>
+  <si>
+    <t>1. Go to cart.
+2. Click on ckeckout.
+3. Enter valid shipping details.
+4. Select the payment method
+5. Place order</t>
+  </si>
+  <si>
+    <t>Order placed successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Order placed successfully, order confirmation shown (email/SMS if configured)</t>
+  </si>
+  <si>
+    <t>Verify checkout cancellation</t>
+  </si>
+  <si>
+    <t>1. Go to Checkout
+2. Click Cancel / Back
+3. Confirm cancellation</t>
+  </si>
+  <si>
+    <t>Checkout canceled, user redirected to cart without placing order</t>
+  </si>
+  <si>
+    <t>Checkout canceled but not redirected to cart page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +692,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,6 +730,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,9 +740,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -711,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF79D45-AEF6-4E71-99A2-CC6D3995BC8D}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,49 +1091,49 @@
     <col min="2" max="2" width="34.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -877,10 +1245,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1039,22 +1407,510 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B36" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>